<commit_message>
Merging new changes to Git
</commit_message>
<xml_diff>
--- a/Indigo Test Cases.xlsx
+++ b/Indigo Test Cases.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Verify that when the user enters the details in Book Flight screen the Flight page opens</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -834,7 +837,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -848,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -862,7 +865,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Test Test Test
</commit_message>
<xml_diff>
--- a/Indigo Test Cases.xlsx
+++ b/Indigo Test Cases.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>Verify that when the user enters the details in Book Flight screen the Flight page opens</t>
   </si>
@@ -823,7 +823,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>